<commit_message>
indicators updated to 2022
</commit_message>
<xml_diff>
--- a/data/analysis/indicators/indic_pivot_tables/indic-accreditation/indic_counts-accreditation.xlsx
+++ b/data/analysis/indicators/indic_pivot_tables/indic-accreditation/indic_counts-accreditation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="31">
   <si>
     <t>session_id</t>
   </si>
@@ -62,6 +62,27 @@
   </si>
   <si>
     <t>20211108</t>
+  </si>
+  <si>
+    <t>20211206</t>
+  </si>
+  <si>
+    <t>20220103</t>
+  </si>
+  <si>
+    <t>20220131</t>
+  </si>
+  <si>
+    <t>20220228</t>
+  </si>
+  <si>
+    <t>20220328</t>
+  </si>
+  <si>
+    <t>20220425</t>
+  </si>
+  <si>
+    <t>20220524</t>
   </si>
   <si>
     <t>closed_cur</t>
@@ -447,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -481,10 +502,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>1274</v>
@@ -504,10 +525,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>976</v>
@@ -527,10 +548,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>686</v>
@@ -550,10 +571,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>429</v>
@@ -573,10 +594,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>1442</v>
@@ -596,10 +617,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>1255</v>
@@ -619,10 +640,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>809</v>
@@ -642,10 +663,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>667</v>
@@ -665,10 +686,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D10">
         <v>1319</v>
@@ -688,10 +709,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>1098</v>
@@ -711,10 +732,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D12">
         <v>774</v>
@@ -734,10 +755,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>580</v>
@@ -757,10 +778,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>1265</v>
@@ -780,10 +801,10 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>988</v>
@@ -803,10 +824,10 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D16">
         <v>717</v>
@@ -826,10 +847,10 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>444</v>
@@ -849,10 +870,10 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>1455</v>
@@ -872,10 +893,10 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>1267</v>
@@ -895,10 +916,10 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D20">
         <v>817</v>
@@ -918,10 +939,10 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>713</v>
@@ -941,10 +962,10 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>1334</v>
@@ -964,10 +985,10 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>1126</v>
@@ -987,10 +1008,10 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D24">
         <v>775</v>
@@ -1010,10 +1031,10 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D25">
         <v>582</v>
@@ -1033,10 +1054,10 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D26">
         <v>1190</v>
@@ -1056,10 +1077,10 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D27">
         <v>956</v>
@@ -1079,10 +1100,10 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D28">
         <v>697</v>
@@ -1102,10 +1123,10 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D29">
         <v>437</v>
@@ -1125,10 +1146,10 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D30">
         <v>1451</v>
@@ -1148,10 +1169,10 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D31">
         <v>1278</v>
@@ -1171,10 +1192,10 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D32">
         <v>876</v>
@@ -1194,10 +1215,10 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D33">
         <v>729</v>
@@ -1217,10 +1238,10 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D34">
         <v>1333</v>
@@ -1240,10 +1261,10 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D35">
         <v>1134</v>
@@ -1263,10 +1284,10 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D36">
         <v>756</v>
@@ -1286,10 +1307,10 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D37">
         <v>603</v>
@@ -1309,10 +1330,10 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D38">
         <v>1074</v>
@@ -1332,10 +1353,10 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D39">
         <v>907</v>
@@ -1355,10 +1376,10 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D40">
         <v>683</v>
@@ -1378,10 +1399,10 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D41">
         <v>439</v>
@@ -1401,10 +1422,10 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D42">
         <v>1452</v>
@@ -1424,10 +1445,10 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D43">
         <v>1278</v>
@@ -1447,10 +1468,10 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D44">
         <v>930</v>
@@ -1470,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D45">
         <v>766</v>
@@ -1493,10 +1514,10 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D46">
         <v>1313</v>
@@ -1516,10 +1537,10 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D47">
         <v>1122</v>
@@ -1539,10 +1560,10 @@
         <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D48">
         <v>758</v>
@@ -1562,10 +1583,10 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D49">
         <v>599</v>
@@ -1585,10 +1606,10 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D50">
         <v>1077</v>
@@ -1608,10 +1629,10 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D51">
         <v>899</v>
@@ -1631,10 +1652,10 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D52">
         <v>682</v>
@@ -1654,10 +1675,10 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D53">
         <v>437</v>
@@ -1677,10 +1698,10 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D54">
         <v>1451</v>
@@ -1700,10 +1721,10 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D55">
         <v>1281</v>
@@ -1723,10 +1744,10 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D56">
         <v>937</v>
@@ -1746,10 +1767,10 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D57">
         <v>765</v>
@@ -1769,10 +1790,10 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C58" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D58">
         <v>1308</v>
@@ -1792,10 +1813,10 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D59">
         <v>1116</v>
@@ -1815,10 +1836,10 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D60">
         <v>765</v>
@@ -1838,10 +1859,10 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D61">
         <v>597</v>
@@ -1861,10 +1882,10 @@
         <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D62">
         <v>1036</v>
@@ -1884,10 +1905,10 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C63" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D63">
         <v>876</v>
@@ -1907,10 +1928,10 @@
         <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C64" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D64">
         <v>673</v>
@@ -1930,10 +1951,10 @@
         <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D65">
         <v>436</v>
@@ -1953,10 +1974,10 @@
         <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C66" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D66">
         <v>1445</v>
@@ -1976,10 +1997,10 @@
         <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D67">
         <v>1278</v>
@@ -1999,10 +2020,10 @@
         <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C68" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D68">
         <v>954</v>
@@ -2022,10 +2043,10 @@
         <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D69">
         <v>781</v>
@@ -2045,10 +2066,10 @@
         <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C70" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D70">
         <v>1281</v>
@@ -2068,10 +2089,10 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D71">
         <v>1106</v>
@@ -2091,10 +2112,10 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D72">
         <v>768</v>
@@ -2114,10 +2135,10 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D73">
         <v>589</v>
@@ -2137,10 +2158,10 @@
         <v>13</v>
       </c>
       <c r="B74" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C74" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D74">
         <v>998</v>
@@ -2160,10 +2181,10 @@
         <v>13</v>
       </c>
       <c r="B75" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D75">
         <v>848</v>
@@ -2183,10 +2204,10 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D76">
         <v>676</v>
@@ -2206,10 +2227,10 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C77" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D77">
         <v>434</v>
@@ -2229,10 +2250,10 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C78" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D78">
         <v>1452</v>
@@ -2252,10 +2273,10 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D79">
         <v>1267</v>
@@ -2275,10 +2296,10 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C80" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D80">
         <v>960</v>
@@ -2298,10 +2319,10 @@
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C81" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D81">
         <v>789</v>
@@ -2321,10 +2342,10 @@
         <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C82" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D82">
         <v>1266</v>
@@ -2344,10 +2365,10 @@
         <v>13</v>
       </c>
       <c r="B83" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C83" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D83">
         <v>1091</v>
@@ -2367,10 +2388,10 @@
         <v>13</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C84" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D84">
         <v>775</v>
@@ -2390,10 +2411,10 @@
         <v>13</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C85" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D85">
         <v>582</v>
@@ -2413,10 +2434,10 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C86" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D86">
         <v>954</v>
@@ -2436,10 +2457,10 @@
         <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D87">
         <v>806</v>
@@ -2459,10 +2480,10 @@
         <v>14</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C88" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D88">
         <v>674</v>
@@ -2482,10 +2503,10 @@
         <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C89" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D89">
         <v>416</v>
@@ -2505,10 +2526,10 @@
         <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C90" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D90">
         <v>1466</v>
@@ -2528,10 +2549,10 @@
         <v>14</v>
       </c>
       <c r="B91" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C91" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D91">
         <v>1292</v>
@@ -2551,10 +2572,10 @@
         <v>14</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C92" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D92">
         <v>978</v>
@@ -2574,10 +2595,10 @@
         <v>14</v>
       </c>
       <c r="B93" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D93">
         <v>797</v>
@@ -2597,10 +2618,10 @@
         <v>14</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C94" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D94">
         <v>1239</v>
@@ -2620,10 +2641,10 @@
         <v>14</v>
       </c>
       <c r="B95" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C95" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D95">
         <v>1066</v>
@@ -2643,10 +2664,10 @@
         <v>14</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C96" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D96">
         <v>763</v>
@@ -2666,10 +2687,10 @@
         <v>14</v>
       </c>
       <c r="B97" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C97" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D97">
         <v>579</v>
@@ -2689,10 +2710,10 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C98" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D98">
         <v>951</v>
@@ -2712,10 +2733,10 @@
         <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C99" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D99">
         <v>805</v>
@@ -2735,10 +2756,10 @@
         <v>15</v>
       </c>
       <c r="B100" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C100" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D100">
         <v>678</v>
@@ -2758,10 +2779,10 @@
         <v>15</v>
       </c>
       <c r="B101" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C101" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D101">
         <v>414</v>
@@ -2781,10 +2802,10 @@
         <v>15</v>
       </c>
       <c r="B102" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C102" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D102">
         <v>1458</v>
@@ -2804,10 +2825,10 @@
         <v>15</v>
       </c>
       <c r="B103" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C103" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D103">
         <v>1280</v>
@@ -2827,10 +2848,10 @@
         <v>15</v>
       </c>
       <c r="B104" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C104" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D104">
         <v>976</v>
@@ -2850,10 +2871,10 @@
         <v>15</v>
       </c>
       <c r="B105" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D105">
         <v>780</v>
@@ -2873,10 +2894,10 @@
         <v>15</v>
       </c>
       <c r="B106" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C106" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D106">
         <v>1218</v>
@@ -2896,10 +2917,10 @@
         <v>15</v>
       </c>
       <c r="B107" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C107" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D107">
         <v>1055</v>
@@ -2919,10 +2940,10 @@
         <v>15</v>
       </c>
       <c r="B108" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C108" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D108">
         <v>759</v>
@@ -2942,10 +2963,10 @@
         <v>15</v>
       </c>
       <c r="B109" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C109" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D109">
         <v>576</v>
@@ -2958,6 +2979,1938 @@
       </c>
       <c r="G109" s="2">
         <v>44508</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>16</v>
+      </c>
+      <c r="B110" t="s">
+        <v>23</v>
+      </c>
+      <c r="C110" t="s">
+        <v>29</v>
+      </c>
+      <c r="D110">
+        <v>942</v>
+      </c>
+      <c r="E110">
+        <v>1651</v>
+      </c>
+      <c r="F110">
+        <v>57.1</v>
+      </c>
+      <c r="G110" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>16</v>
+      </c>
+      <c r="B111" t="s">
+        <v>23</v>
+      </c>
+      <c r="C111" t="s">
+        <v>30</v>
+      </c>
+      <c r="D111">
+        <v>801</v>
+      </c>
+      <c r="E111">
+        <v>1690</v>
+      </c>
+      <c r="F111">
+        <v>47.4</v>
+      </c>
+      <c r="G111" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>16</v>
+      </c>
+      <c r="B112" t="s">
+        <v>24</v>
+      </c>
+      <c r="C112" t="s">
+        <v>29</v>
+      </c>
+      <c r="D112">
+        <v>674</v>
+      </c>
+      <c r="E112">
+        <v>1651</v>
+      </c>
+      <c r="F112">
+        <v>40.8</v>
+      </c>
+      <c r="G112" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>16</v>
+      </c>
+      <c r="B113" t="s">
+        <v>24</v>
+      </c>
+      <c r="C113" t="s">
+        <v>30</v>
+      </c>
+      <c r="D113">
+        <v>418</v>
+      </c>
+      <c r="E113">
+        <v>1690</v>
+      </c>
+      <c r="F113">
+        <v>24.7</v>
+      </c>
+      <c r="G113" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" t="s">
+        <v>25</v>
+      </c>
+      <c r="C114" t="s">
+        <v>29</v>
+      </c>
+      <c r="D114">
+        <v>1455</v>
+      </c>
+      <c r="E114">
+        <v>1651</v>
+      </c>
+      <c r="F114">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="G114" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" t="s">
+        <v>25</v>
+      </c>
+      <c r="C115" t="s">
+        <v>30</v>
+      </c>
+      <c r="D115">
+        <v>1274</v>
+      </c>
+      <c r="E115">
+        <v>1690</v>
+      </c>
+      <c r="F115">
+        <v>75.40000000000001</v>
+      </c>
+      <c r="G115" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" t="s">
+        <v>26</v>
+      </c>
+      <c r="C116" t="s">
+        <v>29</v>
+      </c>
+      <c r="D116">
+        <v>969</v>
+      </c>
+      <c r="E116">
+        <v>1651</v>
+      </c>
+      <c r="F116">
+        <v>58.7</v>
+      </c>
+      <c r="G116" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117" t="s">
+        <v>26</v>
+      </c>
+      <c r="C117" t="s">
+        <v>30</v>
+      </c>
+      <c r="D117">
+        <v>763</v>
+      </c>
+      <c r="E117">
+        <v>1690</v>
+      </c>
+      <c r="F117">
+        <v>45.1</v>
+      </c>
+      <c r="G117" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>16</v>
+      </c>
+      <c r="B118" t="s">
+        <v>27</v>
+      </c>
+      <c r="C118" t="s">
+        <v>29</v>
+      </c>
+      <c r="D118">
+        <v>1205</v>
+      </c>
+      <c r="E118">
+        <v>1651</v>
+      </c>
+      <c r="F118">
+        <v>73</v>
+      </c>
+      <c r="G118" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>16</v>
+      </c>
+      <c r="B119" t="s">
+        <v>27</v>
+      </c>
+      <c r="C119" t="s">
+        <v>30</v>
+      </c>
+      <c r="D119">
+        <v>1040</v>
+      </c>
+      <c r="E119">
+        <v>1690</v>
+      </c>
+      <c r="F119">
+        <v>61.5</v>
+      </c>
+      <c r="G119" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>16</v>
+      </c>
+      <c r="B120" t="s">
+        <v>28</v>
+      </c>
+      <c r="C120" t="s">
+        <v>29</v>
+      </c>
+      <c r="D120">
+        <v>741</v>
+      </c>
+      <c r="E120">
+        <v>1651</v>
+      </c>
+      <c r="F120">
+        <v>44.9</v>
+      </c>
+      <c r="G120" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>16</v>
+      </c>
+      <c r="B121" t="s">
+        <v>28</v>
+      </c>
+      <c r="C121" t="s">
+        <v>30</v>
+      </c>
+      <c r="D121">
+        <v>574</v>
+      </c>
+      <c r="E121">
+        <v>1690</v>
+      </c>
+      <c r="F121">
+        <v>34</v>
+      </c>
+      <c r="G121" s="2">
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>17</v>
+      </c>
+      <c r="B122" t="s">
+        <v>23</v>
+      </c>
+      <c r="C122" t="s">
+        <v>29</v>
+      </c>
+      <c r="D122">
+        <v>1004</v>
+      </c>
+      <c r="E122">
+        <v>1651</v>
+      </c>
+      <c r="F122">
+        <v>60.8</v>
+      </c>
+      <c r="G122" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
+        <v>17</v>
+      </c>
+      <c r="B123" t="s">
+        <v>23</v>
+      </c>
+      <c r="C123" t="s">
+        <v>30</v>
+      </c>
+      <c r="D123">
+        <v>831</v>
+      </c>
+      <c r="E123">
+        <v>1690</v>
+      </c>
+      <c r="F123">
+        <v>49.2</v>
+      </c>
+      <c r="G123" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
+        <v>17</v>
+      </c>
+      <c r="B124" t="s">
+        <v>24</v>
+      </c>
+      <c r="C124" t="s">
+        <v>29</v>
+      </c>
+      <c r="D124">
+        <v>676</v>
+      </c>
+      <c r="E124">
+        <v>1651</v>
+      </c>
+      <c r="F124">
+        <v>40.9</v>
+      </c>
+      <c r="G124" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
+        <v>17</v>
+      </c>
+      <c r="B125" t="s">
+        <v>24</v>
+      </c>
+      <c r="C125" t="s">
+        <v>30</v>
+      </c>
+      <c r="D125">
+        <v>421</v>
+      </c>
+      <c r="E125">
+        <v>1690</v>
+      </c>
+      <c r="F125">
+        <v>24.9</v>
+      </c>
+      <c r="G125" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
+        <v>17</v>
+      </c>
+      <c r="B126" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126" t="s">
+        <v>29</v>
+      </c>
+      <c r="D126">
+        <v>1454</v>
+      </c>
+      <c r="E126">
+        <v>1651</v>
+      </c>
+      <c r="F126">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="G126" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
+        <v>17</v>
+      </c>
+      <c r="B127" t="s">
+        <v>25</v>
+      </c>
+      <c r="C127" t="s">
+        <v>30</v>
+      </c>
+      <c r="D127">
+        <v>1270</v>
+      </c>
+      <c r="E127">
+        <v>1690</v>
+      </c>
+      <c r="F127">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="G127" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
+        <v>17</v>
+      </c>
+      <c r="B128" t="s">
+        <v>26</v>
+      </c>
+      <c r="C128" t="s">
+        <v>29</v>
+      </c>
+      <c r="D128">
+        <v>944</v>
+      </c>
+      <c r="E128">
+        <v>1651</v>
+      </c>
+      <c r="F128">
+        <v>57.2</v>
+      </c>
+      <c r="G128" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
+        <v>17</v>
+      </c>
+      <c r="B129" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129" t="s">
+        <v>30</v>
+      </c>
+      <c r="D129">
+        <v>766</v>
+      </c>
+      <c r="E129">
+        <v>1690</v>
+      </c>
+      <c r="F129">
+        <v>45.3</v>
+      </c>
+      <c r="G129" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
+        <v>17</v>
+      </c>
+      <c r="B130" t="s">
+        <v>27</v>
+      </c>
+      <c r="C130" t="s">
+        <v>29</v>
+      </c>
+      <c r="D130">
+        <v>1220</v>
+      </c>
+      <c r="E130">
+        <v>1651</v>
+      </c>
+      <c r="F130">
+        <v>73.90000000000001</v>
+      </c>
+      <c r="G130" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>17</v>
+      </c>
+      <c r="B131" t="s">
+        <v>27</v>
+      </c>
+      <c r="C131" t="s">
+        <v>30</v>
+      </c>
+      <c r="D131">
+        <v>1059</v>
+      </c>
+      <c r="E131">
+        <v>1690</v>
+      </c>
+      <c r="F131">
+        <v>62.7</v>
+      </c>
+      <c r="G131" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>17</v>
+      </c>
+      <c r="B132" t="s">
+        <v>28</v>
+      </c>
+      <c r="C132" t="s">
+        <v>29</v>
+      </c>
+      <c r="D132">
+        <v>747</v>
+      </c>
+      <c r="E132">
+        <v>1651</v>
+      </c>
+      <c r="F132">
+        <v>45.2</v>
+      </c>
+      <c r="G132" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
+        <v>17</v>
+      </c>
+      <c r="B133" t="s">
+        <v>28</v>
+      </c>
+      <c r="C133" t="s">
+        <v>30</v>
+      </c>
+      <c r="D133">
+        <v>567</v>
+      </c>
+      <c r="E133">
+        <v>1690</v>
+      </c>
+      <c r="F133">
+        <v>33.6</v>
+      </c>
+      <c r="G133" s="2">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" t="s">
+        <v>18</v>
+      </c>
+      <c r="B134" t="s">
+        <v>23</v>
+      </c>
+      <c r="C134" t="s">
+        <v>29</v>
+      </c>
+      <c r="D134">
+        <v>990</v>
+      </c>
+      <c r="E134">
+        <v>1651</v>
+      </c>
+      <c r="F134">
+        <v>60</v>
+      </c>
+      <c r="G134" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" t="s">
+        <v>18</v>
+      </c>
+      <c r="B135" t="s">
+        <v>23</v>
+      </c>
+      <c r="C135" t="s">
+        <v>30</v>
+      </c>
+      <c r="D135">
+        <v>825</v>
+      </c>
+      <c r="E135">
+        <v>1690</v>
+      </c>
+      <c r="F135">
+        <v>48.8</v>
+      </c>
+      <c r="G135" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" t="s">
+        <v>24</v>
+      </c>
+      <c r="C136" t="s">
+        <v>29</v>
+      </c>
+      <c r="D136">
+        <v>674</v>
+      </c>
+      <c r="E136">
+        <v>1651</v>
+      </c>
+      <c r="F136">
+        <v>40.8</v>
+      </c>
+      <c r="G136" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" t="s">
+        <v>18</v>
+      </c>
+      <c r="B137" t="s">
+        <v>24</v>
+      </c>
+      <c r="C137" t="s">
+        <v>30</v>
+      </c>
+      <c r="D137">
+        <v>424</v>
+      </c>
+      <c r="E137">
+        <v>1690</v>
+      </c>
+      <c r="F137">
+        <v>25.1</v>
+      </c>
+      <c r="G137" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" t="s">
+        <v>18</v>
+      </c>
+      <c r="B138" t="s">
+        <v>25</v>
+      </c>
+      <c r="C138" t="s">
+        <v>29</v>
+      </c>
+      <c r="D138">
+        <v>1451</v>
+      </c>
+      <c r="E138">
+        <v>1651</v>
+      </c>
+      <c r="F138">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="G138" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" t="s">
+        <v>18</v>
+      </c>
+      <c r="B139" t="s">
+        <v>25</v>
+      </c>
+      <c r="C139" t="s">
+        <v>30</v>
+      </c>
+      <c r="D139">
+        <v>1271</v>
+      </c>
+      <c r="E139">
+        <v>1690</v>
+      </c>
+      <c r="F139">
+        <v>75.2</v>
+      </c>
+      <c r="G139" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" t="s">
+        <v>18</v>
+      </c>
+      <c r="B140" t="s">
+        <v>26</v>
+      </c>
+      <c r="C140" t="s">
+        <v>29</v>
+      </c>
+      <c r="D140">
+        <v>942</v>
+      </c>
+      <c r="E140">
+        <v>1651</v>
+      </c>
+      <c r="F140">
+        <v>57.1</v>
+      </c>
+      <c r="G140" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" t="s">
+        <v>18</v>
+      </c>
+      <c r="B141" t="s">
+        <v>26</v>
+      </c>
+      <c r="C141" t="s">
+        <v>30</v>
+      </c>
+      <c r="D141">
+        <v>773</v>
+      </c>
+      <c r="E141">
+        <v>1690</v>
+      </c>
+      <c r="F141">
+        <v>45.7</v>
+      </c>
+      <c r="G141" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" t="s">
+        <v>18</v>
+      </c>
+      <c r="B142" t="s">
+        <v>27</v>
+      </c>
+      <c r="C142" t="s">
+        <v>29</v>
+      </c>
+      <c r="D142">
+        <v>1213</v>
+      </c>
+      <c r="E142">
+        <v>1651</v>
+      </c>
+      <c r="F142">
+        <v>73.5</v>
+      </c>
+      <c r="G142" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" t="s">
+        <v>18</v>
+      </c>
+      <c r="B143" t="s">
+        <v>27</v>
+      </c>
+      <c r="C143" t="s">
+        <v>30</v>
+      </c>
+      <c r="D143">
+        <v>1055</v>
+      </c>
+      <c r="E143">
+        <v>1690</v>
+      </c>
+      <c r="F143">
+        <v>62.4</v>
+      </c>
+      <c r="G143" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" t="s">
+        <v>18</v>
+      </c>
+      <c r="B144" t="s">
+        <v>28</v>
+      </c>
+      <c r="C144" t="s">
+        <v>29</v>
+      </c>
+      <c r="D144">
+        <v>745</v>
+      </c>
+      <c r="E144">
+        <v>1651</v>
+      </c>
+      <c r="F144">
+        <v>45.1</v>
+      </c>
+      <c r="G144" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" t="s">
+        <v>18</v>
+      </c>
+      <c r="B145" t="s">
+        <v>28</v>
+      </c>
+      <c r="C145" t="s">
+        <v>30</v>
+      </c>
+      <c r="D145">
+        <v>572</v>
+      </c>
+      <c r="E145">
+        <v>1690</v>
+      </c>
+      <c r="F145">
+        <v>33.8</v>
+      </c>
+      <c r="G145" s="2">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>19</v>
+      </c>
+      <c r="B146" t="s">
+        <v>23</v>
+      </c>
+      <c r="C146" t="s">
+        <v>29</v>
+      </c>
+      <c r="D146">
+        <v>968</v>
+      </c>
+      <c r="E146">
+        <v>1651</v>
+      </c>
+      <c r="F146">
+        <v>58.6</v>
+      </c>
+      <c r="G146" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" t="s">
+        <v>19</v>
+      </c>
+      <c r="B147" t="s">
+        <v>23</v>
+      </c>
+      <c r="C147" t="s">
+        <v>30</v>
+      </c>
+      <c r="D147">
+        <v>811</v>
+      </c>
+      <c r="E147">
+        <v>1690</v>
+      </c>
+      <c r="F147">
+        <v>48</v>
+      </c>
+      <c r="G147" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" t="s">
+        <v>19</v>
+      </c>
+      <c r="B148" t="s">
+        <v>24</v>
+      </c>
+      <c r="C148" t="s">
+        <v>29</v>
+      </c>
+      <c r="D148">
+        <v>672</v>
+      </c>
+      <c r="E148">
+        <v>1651</v>
+      </c>
+      <c r="F148">
+        <v>40.7</v>
+      </c>
+      <c r="G148" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" t="s">
+        <v>19</v>
+      </c>
+      <c r="B149" t="s">
+        <v>24</v>
+      </c>
+      <c r="C149" t="s">
+        <v>30</v>
+      </c>
+      <c r="D149">
+        <v>416</v>
+      </c>
+      <c r="E149">
+        <v>1690</v>
+      </c>
+      <c r="F149">
+        <v>24.6</v>
+      </c>
+      <c r="G149" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>19</v>
+      </c>
+      <c r="B150" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" t="s">
+        <v>29</v>
+      </c>
+      <c r="D150">
+        <v>1452</v>
+      </c>
+      <c r="E150">
+        <v>1651</v>
+      </c>
+      <c r="F150">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="G150" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" t="s">
+        <v>19</v>
+      </c>
+      <c r="B151" t="s">
+        <v>25</v>
+      </c>
+      <c r="C151" t="s">
+        <v>30</v>
+      </c>
+      <c r="D151">
+        <v>1278</v>
+      </c>
+      <c r="E151">
+        <v>1690</v>
+      </c>
+      <c r="F151">
+        <v>75.59999999999999</v>
+      </c>
+      <c r="G151" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" t="s">
+        <v>19</v>
+      </c>
+      <c r="B152" t="s">
+        <v>26</v>
+      </c>
+      <c r="C152" t="s">
+        <v>29</v>
+      </c>
+      <c r="D152">
+        <v>944</v>
+      </c>
+      <c r="E152">
+        <v>1651</v>
+      </c>
+      <c r="F152">
+        <v>57.2</v>
+      </c>
+      <c r="G152" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" t="s">
+        <v>19</v>
+      </c>
+      <c r="B153" t="s">
+        <v>26</v>
+      </c>
+      <c r="C153" t="s">
+        <v>30</v>
+      </c>
+      <c r="D153">
+        <v>767</v>
+      </c>
+      <c r="E153">
+        <v>1690</v>
+      </c>
+      <c r="F153">
+        <v>45.4</v>
+      </c>
+      <c r="G153" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" t="s">
+        <v>19</v>
+      </c>
+      <c r="B154" t="s">
+        <v>27</v>
+      </c>
+      <c r="C154" t="s">
+        <v>29</v>
+      </c>
+      <c r="D154">
+        <v>1212</v>
+      </c>
+      <c r="E154">
+        <v>1651</v>
+      </c>
+      <c r="F154">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="G154" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" t="s">
+        <v>19</v>
+      </c>
+      <c r="B155" t="s">
+        <v>27</v>
+      </c>
+      <c r="C155" t="s">
+        <v>30</v>
+      </c>
+      <c r="D155">
+        <v>1054</v>
+      </c>
+      <c r="E155">
+        <v>1690</v>
+      </c>
+      <c r="F155">
+        <v>62.4</v>
+      </c>
+      <c r="G155" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" t="s">
+        <v>19</v>
+      </c>
+      <c r="B156" t="s">
+        <v>28</v>
+      </c>
+      <c r="C156" t="s">
+        <v>29</v>
+      </c>
+      <c r="D156">
+        <v>749</v>
+      </c>
+      <c r="E156">
+        <v>1651</v>
+      </c>
+      <c r="F156">
+        <v>45.4</v>
+      </c>
+      <c r="G156" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" t="s">
+        <v>19</v>
+      </c>
+      <c r="B157" t="s">
+        <v>28</v>
+      </c>
+      <c r="C157" t="s">
+        <v>30</v>
+      </c>
+      <c r="D157">
+        <v>571</v>
+      </c>
+      <c r="E157">
+        <v>1690</v>
+      </c>
+      <c r="F157">
+        <v>33.8</v>
+      </c>
+      <c r="G157" s="2">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158" t="s">
+        <v>23</v>
+      </c>
+      <c r="C158" t="s">
+        <v>29</v>
+      </c>
+      <c r="D158">
+        <v>964</v>
+      </c>
+      <c r="E158">
+        <v>1651</v>
+      </c>
+      <c r="F158">
+        <v>58.4</v>
+      </c>
+      <c r="G158" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" t="s">
+        <v>20</v>
+      </c>
+      <c r="B159" t="s">
+        <v>23</v>
+      </c>
+      <c r="C159" t="s">
+        <v>30</v>
+      </c>
+      <c r="D159">
+        <v>794</v>
+      </c>
+      <c r="E159">
+        <v>1690</v>
+      </c>
+      <c r="F159">
+        <v>47</v>
+      </c>
+      <c r="G159" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" t="s">
+        <v>20</v>
+      </c>
+      <c r="B160" t="s">
+        <v>24</v>
+      </c>
+      <c r="C160" t="s">
+        <v>29</v>
+      </c>
+      <c r="D160">
+        <v>670</v>
+      </c>
+      <c r="E160">
+        <v>1651</v>
+      </c>
+      <c r="F160">
+        <v>40.6</v>
+      </c>
+      <c r="G160" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" t="s">
+        <v>20</v>
+      </c>
+      <c r="B161" t="s">
+        <v>24</v>
+      </c>
+      <c r="C161" t="s">
+        <v>30</v>
+      </c>
+      <c r="D161">
+        <v>413</v>
+      </c>
+      <c r="E161">
+        <v>1690</v>
+      </c>
+      <c r="F161">
+        <v>24.4</v>
+      </c>
+      <c r="G161" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" t="s">
+        <v>20</v>
+      </c>
+      <c r="B162" t="s">
+        <v>25</v>
+      </c>
+      <c r="C162" t="s">
+        <v>29</v>
+      </c>
+      <c r="D162">
+        <v>1455</v>
+      </c>
+      <c r="E162">
+        <v>1651</v>
+      </c>
+      <c r="F162">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="G162" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" t="s">
+        <v>20</v>
+      </c>
+      <c r="B163" t="s">
+        <v>25</v>
+      </c>
+      <c r="C163" t="s">
+        <v>30</v>
+      </c>
+      <c r="D163">
+        <v>1270</v>
+      </c>
+      <c r="E163">
+        <v>1690</v>
+      </c>
+      <c r="F163">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="G163" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" t="s">
+        <v>20</v>
+      </c>
+      <c r="B164" t="s">
+        <v>26</v>
+      </c>
+      <c r="C164" t="s">
+        <v>29</v>
+      </c>
+      <c r="D164">
+        <v>944</v>
+      </c>
+      <c r="E164">
+        <v>1651</v>
+      </c>
+      <c r="F164">
+        <v>57.2</v>
+      </c>
+      <c r="G164" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" t="s">
+        <v>20</v>
+      </c>
+      <c r="B165" t="s">
+        <v>26</v>
+      </c>
+      <c r="C165" t="s">
+        <v>30</v>
+      </c>
+      <c r="D165">
+        <v>764</v>
+      </c>
+      <c r="E165">
+        <v>1690</v>
+      </c>
+      <c r="F165">
+        <v>45.2</v>
+      </c>
+      <c r="G165" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" t="s">
+        <v>20</v>
+      </c>
+      <c r="B166" t="s">
+        <v>27</v>
+      </c>
+      <c r="C166" t="s">
+        <v>29</v>
+      </c>
+      <c r="D166">
+        <v>1213</v>
+      </c>
+      <c r="E166">
+        <v>1651</v>
+      </c>
+      <c r="F166">
+        <v>73.5</v>
+      </c>
+      <c r="G166" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" t="s">
+        <v>20</v>
+      </c>
+      <c r="B167" t="s">
+        <v>27</v>
+      </c>
+      <c r="C167" t="s">
+        <v>30</v>
+      </c>
+      <c r="D167">
+        <v>1049</v>
+      </c>
+      <c r="E167">
+        <v>1690</v>
+      </c>
+      <c r="F167">
+        <v>62.1</v>
+      </c>
+      <c r="G167" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
+      <c r="A168" t="s">
+        <v>20</v>
+      </c>
+      <c r="B168" t="s">
+        <v>28</v>
+      </c>
+      <c r="C168" t="s">
+        <v>29</v>
+      </c>
+      <c r="D168">
+        <v>740</v>
+      </c>
+      <c r="E168">
+        <v>1651</v>
+      </c>
+      <c r="F168">
+        <v>44.8</v>
+      </c>
+      <c r="G168" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" t="s">
+        <v>20</v>
+      </c>
+      <c r="B169" t="s">
+        <v>28</v>
+      </c>
+      <c r="C169" t="s">
+        <v>30</v>
+      </c>
+      <c r="D169">
+        <v>568</v>
+      </c>
+      <c r="E169">
+        <v>1690</v>
+      </c>
+      <c r="F169">
+        <v>33.6</v>
+      </c>
+      <c r="G169" s="2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="A170" t="s">
+        <v>21</v>
+      </c>
+      <c r="B170" t="s">
+        <v>23</v>
+      </c>
+      <c r="C170" t="s">
+        <v>29</v>
+      </c>
+      <c r="D170">
+        <v>946</v>
+      </c>
+      <c r="E170">
+        <v>1651</v>
+      </c>
+      <c r="F170">
+        <v>57.3</v>
+      </c>
+      <c r="G170" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7">
+      <c r="A171" t="s">
+        <v>21</v>
+      </c>
+      <c r="B171" t="s">
+        <v>23</v>
+      </c>
+      <c r="C171" t="s">
+        <v>30</v>
+      </c>
+      <c r="D171">
+        <v>782</v>
+      </c>
+      <c r="E171">
+        <v>1690</v>
+      </c>
+      <c r="F171">
+        <v>46.3</v>
+      </c>
+      <c r="G171" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
+      <c r="A172" t="s">
+        <v>21</v>
+      </c>
+      <c r="B172" t="s">
+        <v>24</v>
+      </c>
+      <c r="C172" t="s">
+        <v>29</v>
+      </c>
+      <c r="D172">
+        <v>664</v>
+      </c>
+      <c r="E172">
+        <v>1651</v>
+      </c>
+      <c r="F172">
+        <v>40.2</v>
+      </c>
+      <c r="G172" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
+      <c r="A173" t="s">
+        <v>21</v>
+      </c>
+      <c r="B173" t="s">
+        <v>24</v>
+      </c>
+      <c r="C173" t="s">
+        <v>30</v>
+      </c>
+      <c r="D173">
+        <v>411</v>
+      </c>
+      <c r="E173">
+        <v>1690</v>
+      </c>
+      <c r="F173">
+        <v>24.3</v>
+      </c>
+      <c r="G173" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
+      <c r="A174" t="s">
+        <v>21</v>
+      </c>
+      <c r="B174" t="s">
+        <v>25</v>
+      </c>
+      <c r="C174" t="s">
+        <v>29</v>
+      </c>
+      <c r="D174">
+        <v>1451</v>
+      </c>
+      <c r="E174">
+        <v>1651</v>
+      </c>
+      <c r="F174">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="G174" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
+      <c r="A175" t="s">
+        <v>21</v>
+      </c>
+      <c r="B175" t="s">
+        <v>25</v>
+      </c>
+      <c r="C175" t="s">
+        <v>30</v>
+      </c>
+      <c r="D175">
+        <v>1275</v>
+      </c>
+      <c r="E175">
+        <v>1690</v>
+      </c>
+      <c r="F175">
+        <v>75.40000000000001</v>
+      </c>
+      <c r="G175" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
+      <c r="A176" t="s">
+        <v>21</v>
+      </c>
+      <c r="B176" t="s">
+        <v>26</v>
+      </c>
+      <c r="C176" t="s">
+        <v>29</v>
+      </c>
+      <c r="D176">
+        <v>935</v>
+      </c>
+      <c r="E176">
+        <v>1651</v>
+      </c>
+      <c r="F176">
+        <v>56.6</v>
+      </c>
+      <c r="G176" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
+      <c r="A177" t="s">
+        <v>21</v>
+      </c>
+      <c r="B177" t="s">
+        <v>26</v>
+      </c>
+      <c r="C177" t="s">
+        <v>30</v>
+      </c>
+      <c r="D177">
+        <v>764</v>
+      </c>
+      <c r="E177">
+        <v>1690</v>
+      </c>
+      <c r="F177">
+        <v>45.2</v>
+      </c>
+      <c r="G177" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
+      <c r="A178" t="s">
+        <v>21</v>
+      </c>
+      <c r="B178" t="s">
+        <v>27</v>
+      </c>
+      <c r="C178" t="s">
+        <v>29</v>
+      </c>
+      <c r="D178">
+        <v>1206</v>
+      </c>
+      <c r="E178">
+        <v>1651</v>
+      </c>
+      <c r="F178">
+        <v>73</v>
+      </c>
+      <c r="G178" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" t="s">
+        <v>21</v>
+      </c>
+      <c r="B179" t="s">
+        <v>27</v>
+      </c>
+      <c r="C179" t="s">
+        <v>30</v>
+      </c>
+      <c r="D179">
+        <v>1045</v>
+      </c>
+      <c r="E179">
+        <v>1690</v>
+      </c>
+      <c r="F179">
+        <v>61.8</v>
+      </c>
+      <c r="G179" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7">
+      <c r="A180" t="s">
+        <v>21</v>
+      </c>
+      <c r="B180" t="s">
+        <v>28</v>
+      </c>
+      <c r="C180" t="s">
+        <v>29</v>
+      </c>
+      <c r="D180">
+        <v>730</v>
+      </c>
+      <c r="E180">
+        <v>1651</v>
+      </c>
+      <c r="F180">
+        <v>44.2</v>
+      </c>
+      <c r="G180" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7">
+      <c r="A181" t="s">
+        <v>21</v>
+      </c>
+      <c r="B181" t="s">
+        <v>28</v>
+      </c>
+      <c r="C181" t="s">
+        <v>30</v>
+      </c>
+      <c r="D181">
+        <v>573</v>
+      </c>
+      <c r="E181">
+        <v>1690</v>
+      </c>
+      <c r="F181">
+        <v>33.9</v>
+      </c>
+      <c r="G181" s="2">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7">
+      <c r="A182" t="s">
+        <v>22</v>
+      </c>
+      <c r="B182" t="s">
+        <v>23</v>
+      </c>
+      <c r="C182" t="s">
+        <v>29</v>
+      </c>
+      <c r="D182">
+        <v>944</v>
+      </c>
+      <c r="E182">
+        <v>1651</v>
+      </c>
+      <c r="F182">
+        <v>57.2</v>
+      </c>
+      <c r="G182" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7">
+      <c r="A183" t="s">
+        <v>22</v>
+      </c>
+      <c r="B183" t="s">
+        <v>23</v>
+      </c>
+      <c r="C183" t="s">
+        <v>30</v>
+      </c>
+      <c r="D183">
+        <v>770</v>
+      </c>
+      <c r="E183">
+        <v>1690</v>
+      </c>
+      <c r="F183">
+        <v>45.6</v>
+      </c>
+      <c r="G183" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7">
+      <c r="A184" t="s">
+        <v>22</v>
+      </c>
+      <c r="B184" t="s">
+        <v>24</v>
+      </c>
+      <c r="C184" t="s">
+        <v>29</v>
+      </c>
+      <c r="D184">
+        <v>664</v>
+      </c>
+      <c r="E184">
+        <v>1651</v>
+      </c>
+      <c r="F184">
+        <v>40.2</v>
+      </c>
+      <c r="G184" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7">
+      <c r="A185" t="s">
+        <v>22</v>
+      </c>
+      <c r="B185" t="s">
+        <v>24</v>
+      </c>
+      <c r="C185" t="s">
+        <v>30</v>
+      </c>
+      <c r="D185">
+        <v>411</v>
+      </c>
+      <c r="E185">
+        <v>1690</v>
+      </c>
+      <c r="F185">
+        <v>24.3</v>
+      </c>
+      <c r="G185" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7">
+      <c r="A186" t="s">
+        <v>22</v>
+      </c>
+      <c r="B186" t="s">
+        <v>25</v>
+      </c>
+      <c r="C186" t="s">
+        <v>29</v>
+      </c>
+      <c r="D186">
+        <v>1451</v>
+      </c>
+      <c r="E186">
+        <v>1651</v>
+      </c>
+      <c r="F186">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="G186" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" t="s">
+        <v>22</v>
+      </c>
+      <c r="B187" t="s">
+        <v>25</v>
+      </c>
+      <c r="C187" t="s">
+        <v>30</v>
+      </c>
+      <c r="D187">
+        <v>1272</v>
+      </c>
+      <c r="E187">
+        <v>1690</v>
+      </c>
+      <c r="F187">
+        <v>75.3</v>
+      </c>
+      <c r="G187" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7">
+      <c r="A188" t="s">
+        <v>22</v>
+      </c>
+      <c r="B188" t="s">
+        <v>26</v>
+      </c>
+      <c r="C188" t="s">
+        <v>29</v>
+      </c>
+      <c r="D188">
+        <v>942</v>
+      </c>
+      <c r="E188">
+        <v>1651</v>
+      </c>
+      <c r="F188">
+        <v>57.1</v>
+      </c>
+      <c r="G188" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7">
+      <c r="A189" t="s">
+        <v>22</v>
+      </c>
+      <c r="B189" t="s">
+        <v>26</v>
+      </c>
+      <c r="C189" t="s">
+        <v>30</v>
+      </c>
+      <c r="D189">
+        <v>763</v>
+      </c>
+      <c r="E189">
+        <v>1690</v>
+      </c>
+      <c r="F189">
+        <v>45.1</v>
+      </c>
+      <c r="G189" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7">
+      <c r="A190" t="s">
+        <v>22</v>
+      </c>
+      <c r="B190" t="s">
+        <v>27</v>
+      </c>
+      <c r="C190" t="s">
+        <v>29</v>
+      </c>
+      <c r="D190">
+        <v>1202</v>
+      </c>
+      <c r="E190">
+        <v>1651</v>
+      </c>
+      <c r="F190">
+        <v>72.8</v>
+      </c>
+      <c r="G190" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7">
+      <c r="A191" t="s">
+        <v>22</v>
+      </c>
+      <c r="B191" t="s">
+        <v>27</v>
+      </c>
+      <c r="C191" t="s">
+        <v>30</v>
+      </c>
+      <c r="D191">
+        <v>1038</v>
+      </c>
+      <c r="E191">
+        <v>1690</v>
+      </c>
+      <c r="F191">
+        <v>61.4</v>
+      </c>
+      <c r="G191" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7">
+      <c r="A192" t="s">
+        <v>22</v>
+      </c>
+      <c r="B192" t="s">
+        <v>28</v>
+      </c>
+      <c r="C192" t="s">
+        <v>29</v>
+      </c>
+      <c r="D192">
+        <v>732</v>
+      </c>
+      <c r="E192">
+        <v>1651</v>
+      </c>
+      <c r="F192">
+        <v>44.3</v>
+      </c>
+      <c r="G192" s="2">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7">
+      <c r="A193" t="s">
+        <v>22</v>
+      </c>
+      <c r="B193" t="s">
+        <v>28</v>
+      </c>
+      <c r="C193" t="s">
+        <v>30</v>
+      </c>
+      <c r="D193">
+        <v>570</v>
+      </c>
+      <c r="E193">
+        <v>1690</v>
+      </c>
+      <c r="F193">
+        <v>33.7</v>
+      </c>
+      <c r="G193" s="2">
+        <v>44705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>